<commit_message>
data_in: update of external input data for projection of energy demand.
</commit_message>
<xml_diff>
--- a/data_in/temporal/Activity_drivers.xlsx
+++ b/data_in/temporal/Activity_drivers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" tabRatio="808"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" tabRatio="808" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="drivers_industry_emp" sheetId="15" r:id="rId1"/>
@@ -787,7 +787,7 @@
   </sheetPr>
   <dimension ref="A1:AM91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
@@ -19131,11 +19131,11 @@
   </sheetPr>
   <dimension ref="A1:BH38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AV6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BH2" sqref="BH2"/>
+      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19537,13 +19537,13 @@
         <v>73535084.801312208</v>
       </c>
       <c r="L3" s="14">
-        <v>46762725.277367339</v>
+        <v>47898023.713390075</v>
       </c>
       <c r="M3" s="14">
-        <v>98843997.542914972</v>
+        <v>101243717.30165665</v>
       </c>
       <c r="N3" s="14">
-        <v>170806517.13718936</v>
+        <v>174953332.16172335</v>
       </c>
       <c r="O3" s="14">
         <v>35100782.570857525</v>
@@ -19716,13 +19716,13 @@
         <v>75358640.534865737</v>
       </c>
       <c r="L4" s="14">
-        <v>47865728.179794475</v>
+        <v>49011764.200447783</v>
       </c>
       <c r="M4" s="14">
-        <v>100155054.85304378</v>
+        <v>102553039.90157267</v>
       </c>
       <c r="N4" s="14">
-        <v>174699872.03738812</v>
+        <v>178882663.22791022</v>
       </c>
       <c r="O4" s="14">
         <v>36265065.201097913</v>
@@ -19895,13 +19895,13 @@
         <v>77441568.880353317</v>
       </c>
       <c r="L5" s="14">
-        <v>49179650.310477085</v>
+        <v>50340669.319839202</v>
       </c>
       <c r="M5" s="14">
-        <v>101858666.45210552</v>
+        <v>104263316.49074103</v>
       </c>
       <c r="N5" s="14">
-        <v>178043449.48195985</v>
+        <v>182246647.91944286</v>
       </c>
       <c r="O5" s="14">
         <v>37459223.748321265</v>
@@ -20074,13 +20074,13 @@
         <v>79818634.642518893</v>
       </c>
       <c r="L6" s="19">
-        <v>50144374.817656659</v>
+        <v>51311375.175877109</v>
       </c>
       <c r="M6" s="19">
-        <v>104165952.17436765</v>
+        <v>106590186.2772736</v>
       </c>
       <c r="N6" s="19">
-        <v>180875501.80696985</v>
+        <v>185084982.45499086</v>
       </c>
       <c r="O6" s="19">
         <v>38743288.716540419</v>
@@ -20254,13 +20254,13 @@
         <v>82110936.692681193</v>
       </c>
       <c r="L7" s="19">
-        <v>50869789.087423593</v>
+        <v>52036640.912053317</v>
       </c>
       <c r="M7" s="19">
-        <v>105983152.67742632</v>
+        <v>108414195.48889023</v>
       </c>
       <c r="N7" s="19">
-        <v>182648297.23808256</v>
+        <v>186837886.043562</v>
       </c>
       <c r="O7" s="19">
         <v>40266653.507344171</v>
@@ -20434,13 +20434,13 @@
         <v>82254279.623275399</v>
       </c>
       <c r="L8" s="19">
-        <v>51029579.066053785</v>
+        <v>52183017.287997983</v>
       </c>
       <c r="M8" s="19">
-        <v>106528907.33685562</v>
+        <v>108936814.9800919</v>
       </c>
       <c r="N8" s="19">
-        <v>183222024.16001564</v>
+        <v>187363451.34080014</v>
       </c>
       <c r="O8" s="19">
         <v>40430285.988840893</v>
@@ -20614,13 +20614,13 @@
         <v>82397872.790885255</v>
       </c>
       <c r="L9" s="19">
-        <v>51189870.970045358</v>
+        <v>52329805.413107462</v>
       </c>
       <c r="M9" s="19">
-        <v>107077472.33114254</v>
+        <v>109461953.8012702</v>
       </c>
       <c r="N9" s="19">
-        <v>183797553.24811146</v>
+        <v>187890495.0260008</v>
       </c>
       <c r="O9" s="19">
         <v>40594583.427235402</v>
@@ -20794,13 +20794,13 @@
         <v>82541716.632355228</v>
       </c>
       <c r="L10" s="19">
-        <v>51350666.376024514</v>
+        <v>52477006.445610806</v>
       </c>
       <c r="M10" s="19">
-        <v>107628862.13195835</v>
+        <v>109989624.09706117</v>
       </c>
       <c r="N10" s="19">
-        <v>184374890.16325623</v>
+        <v>188419021.25779265</v>
       </c>
       <c r="O10" s="19">
         <v>40759548.524727613</v>
@@ -20974,13 +20974,13 @@
         <v>82685811.585292414</v>
       </c>
       <c r="L11" s="19">
-        <v>51511966.865569875</v>
+        <v>52624621.546995163</v>
       </c>
       <c r="M11" s="19">
-        <v>108183091.28549533</v>
+        <v>110519838.07064515</v>
       </c>
       <c r="N11" s="19">
-        <v>184954040.58411798</v>
+        <v>188949034.20650262</v>
       </c>
       <c r="O11" s="19">
         <v>40925183.994498439</v>
@@ -21154,13 +21154,13 @@
         <v>82830158.088067755</v>
       </c>
       <c r="L12" s="19">
-        <v>51673774.025228098</v>
+        <v>52772651.882014826</v>
       </c>
       <c r="M12" s="19">
-        <v>108740174.41285074</v>
+        <v>111052607.98402885</v>
       </c>
       <c r="N12" s="19">
-        <v>185535010.2072024</v>
+        <v>189480538.05418831</v>
       </c>
       <c r="O12" s="19">
         <v>41091492.560754351</v>
@@ -21334,13 +21334,13 @@
         <v>82974756.579817548</v>
       </c>
       <c r="L13" s="19">
-        <v>51836089.446529381</v>
+        <v>52921098.618700489</v>
       </c>
       <c r="M13" s="19">
-        <v>109300126.21041235</v>
+        <v>111587946.15832892</v>
       </c>
       <c r="N13" s="19">
-        <v>186117804.74690872</v>
+        <v>190013536.99467126</v>
       </c>
       <c r="O13" s="19">
         <v>41258476.958772279</v>
@@ -21514,13 +21514,13 @@
         <v>83119607.500444695</v>
       </c>
       <c r="L14" s="19">
-        <v>51998914.7260032</v>
+        <v>53069962.928368501</v>
       </c>
       <c r="M14" s="19">
-        <v>109862961.45024619</v>
+        <v>112125864.97405709</v>
       </c>
       <c r="N14" s="19">
-        <v>186702429.93558601</v>
+        <v>190548035.23357016</v>
       </c>
       <c r="O14" s="19">
         <v>41426139.934944563</v>
@@ -21694,13 +21694,13 @@
         <v>83264711.290620014</v>
       </c>
       <c r="L15" s="19">
-        <v>52162251.465193942</v>
+        <v>53219245.985630043</v>
       </c>
       <c r="M15" s="19">
-        <v>110428694.98048626</v>
+        <v>112666376.87140633</v>
       </c>
       <c r="N15" s="19">
-        <v>187288891.52358946</v>
+        <v>191084036.98833379</v>
       </c>
       <c r="O15" s="19">
         <v>41594484.246824101</v>
@@ -21874,13 +21874,13 @@
         <v>83410068.39178364</v>
       </c>
       <c r="L16" s="19">
-        <v>52326101.270676754</v>
+        <v>53368948.968400396</v>
       </c>
       <c r="M16" s="19">
-        <v>110997341.72572632</v>
+        <v>113209494.35053854</v>
       </c>
       <c r="N16" s="19">
-        <v>187877195.27933717</v>
+        <v>191621546.4882744</v>
       </c>
       <c r="O16" s="19">
         <v>41763512.663169719</v>
@@ -22054,13 +22054,13 @@
         <v>83555679.246146306</v>
       </c>
       <c r="L17" s="19">
-        <v>52490465.754073255</v>
+        <v>53519073.057908282</v>
       </c>
       <c r="M17" s="19">
-        <v>111568916.6874135</v>
+        <v>113755229.97187372</v>
       </c>
       <c r="N17" s="19">
-        <v>188467346.98936677</v>
+        <v>192160567.97460121</v>
       </c>
       <c r="O17" s="19">
         <v>41933227.963991724</v>
@@ -22234,13 +22234,13 @@
         <v>83701544.296690777</v>
       </c>
       <c r="L18" s="19">
-        <v>52655346.532067411</v>
+        <v>53669619.438705109</v>
       </c>
       <c r="M18" s="19">
-        <v>112143434.94424401</v>
+        <v>114303596.35638025</v>
       </c>
       <c r="N18" s="19">
-        <v>189059352.45839217</v>
+        <v>192701105.7004534</v>
       </c>
       <c r="O18" s="19">
         <v>42103632.940597594</v>
@@ -22414,13 +22414,13 @@
         <v>83847663.987173125</v>
       </c>
       <c r="L19" s="19">
-        <v>52820745.226421431</v>
+        <v>53820589.298674464</v>
       </c>
       <c r="M19" s="19">
-        <v>112720911.6525611</v>
+        <v>114854606.18586722</v>
       </c>
       <c r="N19" s="19">
-        <v>189653217.50936073</v>
+        <v>193243163.93093446</v>
       </c>
       <c r="O19" s="19">
         <v>42274730.395637929</v>
@@ -22594,13 +22594,13 @@
         <v>83994038.762124047</v>
       </c>
       <c r="L20" s="19">
-        <v>52986663.463991791</v>
+        <v>53971983.829041272</v>
       </c>
       <c r="M20" s="19">
-        <v>113301362.04675481</v>
+        <v>115408272.2032771</v>
       </c>
       <c r="N20" s="19">
-        <v>190248947.98351088</v>
+        <v>193786746.94314501</v>
       </c>
       <c r="O20" s="19">
         <v>42446523.143152483</v>
@@ -22774,13 +22774,13 @@
         <v>84140669.066850305</v>
       </c>
       <c r="L21" s="19">
-        <v>53153102.87674512</v>
+        <v>54123804.224381365</v>
       </c>
       <c r="M21" s="19">
-        <v>113884801.43966386</v>
+        <v>115964607.21298088</v>
       </c>
       <c r="N21" s="19">
-        <v>190846549.7404291</v>
+        <v>194331859.02621707</v>
       </c>
       <c r="O21" s="19">
         <v>42619014.008616515</v>
@@ -22954,13 +22954,13 @@
         <v>84287555.347436041</v>
       </c>
       <c r="L22" s="19">
-        <v>53320065.10177435</v>
+        <v>54276051.682630897</v>
       </c>
       <c r="M22" s="19">
-        <v>114471245.22297961</v>
+        <v>116523624.08107418</v>
       </c>
       <c r="N22" s="19">
-        <v>191446028.65810779</v>
+        <v>194878504.48134789</v>
       </c>
       <c r="O22" s="19">
         <v>42792205.828987226</v>
@@ -23134,13 +23134,13 @@
         <v>84434698.050744161</v>
       </c>
       <c r="L23" s="19">
-        <v>53487551.781314746</v>
+        <v>54428727.405095704</v>
       </c>
       <c r="M23" s="19">
-        <v>115060708.86765206</v>
+        <v>117085335.73567452</v>
       </c>
       <c r="N23" s="19">
-        <v>192047390.63300291</v>
+        <v>195426687.62183359</v>
       </c>
       <c r="O23" s="19">
         <v>42966101.452750422</v>
@@ -23314,13 +23314,13 @@
         <v>84582097.624417618</v>
       </c>
       <c r="L24" s="19">
-        <v>53655564.562760122</v>
+        <v>54581832.596460819</v>
       </c>
       <c r="M24" s="19">
-        <v>115653207.92429823</v>
+        <v>117649755.16722052</v>
       </c>
       <c r="N24" s="19">
-        <v>192650641.5800924</v>
+        <v>195976412.77310342</v>
       </c>
       <c r="O24" s="19">
         <v>43140703.739967339</v>
@@ -23494,13 +23494,13 @@
         <v>84729754.51688087</v>
       </c>
       <c r="L25" s="19">
-        <v>53824105.098678991</v>
+        <v>54735368.464800045</v>
       </c>
       <c r="M25" s="19">
-        <v>116248758.02361204</v>
+        <v>118216895.42877232</v>
       </c>
       <c r="N25" s="19">
-        <v>193255787.43293393</v>
+        <v>196527684.27275395</v>
       </c>
       <c r="O25" s="19">
         <v>43316015.562321745</v>
@@ -23674,13 +23674,13 @@
         <v>84877669.177341193</v>
       </c>
       <c r="L26" s="19">
-        <v>53993175.04683087</v>
+        <v>54889336.221585378</v>
       </c>
       <c r="M26" s="19">
-        <v>116847374.87677698</v>
+        <v>118786769.63631333</v>
       </c>
       <c r="N26" s="19">
-        <v>193862834.14372331</v>
+        <v>197080506.47058296</v>
       </c>
       <c r="O26" s="19">
         <v>43492039.803167105</v>
@@ -23854,13 +23854,13 @@
         <v>85025842.055790052</v>
       </c>
       <c r="L27" s="19">
-        <v>54162776.070182502</v>
+        <v>55043737.081696682</v>
       </c>
       <c r="M27" s="19">
-        <v>117449074.27588029</v>
+        <v>119359390.96905373</v>
       </c>
       <c r="N27" s="19">
-        <v>194471787.68335322</v>
+        <v>197634883.72862431</v>
       </c>
       <c r="O27" s="19">
         <v>43668779.357574046</v>
@@ -24034,13 +24034,13 @@
         <v>85174273.603004441</v>
       </c>
       <c r="L28" s="19">
-        <v>54332909.836924344</v>
+        <v>55198572.263431177</v>
       </c>
       <c r="M28" s="19">
-        <v>118053872.09432994</v>
+        <v>119934772.66973504</v>
       </c>
       <c r="N28" s="19">
-        <v>195082654.0414719</v>
+        <v>198190820.42118174</v>
       </c>
       <c r="O28" s="19">
         <v>43846237.132377952</v>
@@ -24214,13 +24214,13 @@
         <v>85322964.270548299</v>
       </c>
       <c r="L29" s="19">
-        <v>54503578.020486854</v>
+        <v>55353842.98851306</v>
       </c>
       <c r="M29" s="19">
-        <v>118661784.28727299</v>
+        <v>120512928.04493651</v>
       </c>
       <c r="N29" s="19">
-        <v>195695439.22654191</v>
+        <v>198748320.93486363</v>
       </c>
       <c r="O29" s="19">
         <v>44024416.046226747</v>
@@ -24394,13 +24394,13 @@
         <v>85471914.510773912</v>
       </c>
       <c r="L30" s="19">
-        <v>54674782.299557008</v>
+        <v>55509550.482103258</v>
       </c>
       <c r="M30" s="19">
-        <v>119272826.89201681</v>
+        <v>121093870.46538298</v>
       </c>
       <c r="N30" s="19">
-        <v>196310149.26589939</v>
+        <v>199307389.66861799</v>
       </c>
       <c r="O30" s="19">
         <v>44203319.029628992</v>
@@ -24574,13 +24574,13 @@
         <v>85621124.776823208</v>
       </c>
       <c r="L31" s="19">
-        <v>54846524.358094782</v>
+        <v>55665695.972808935</v>
       </c>
       <c r="M31" s="19">
-        <v>119887016.02845196</v>
+        <v>121677613.36625381</v>
       </c>
       <c r="N31" s="19">
-        <v>196926790.2058132</v>
+        <v>199868031.03376666</v>
       </c>
       <c r="O31" s="19">
         <v>44382949.025001965</v>
@@ -24754,13 +24754,13 @@
         <v>85770595.522629172</v>
       </c>
       <c r="L32" s="19">
-        <v>55018805.885349758</v>
+        <v>55822280.692693301</v>
       </c>
       <c r="M32" s="19">
-        <v>120504367.89947757</v>
+        <v>122264170.2474938</v>
       </c>
       <c r="N32" s="19">
-        <v>197545368.11154464</v>
+        <v>200430249.45404023</v>
       </c>
       <c r="O32" s="19">
         <v>44563308.986720145</v>
@@ -24934,13 +24934,13 @@
         <v>85920327.202917263</v>
       </c>
       <c r="L33" s="19">
-        <v>55191628.575877741</v>
+        <v>55979305.877285294</v>
       </c>
       <c r="M33" s="19">
-        <v>121124898.7914288</v>
+        <v>122853554.67412539</v>
       </c>
       <c r="N33" s="19">
-        <v>198165889.06740692</v>
+        <v>200994049.36561319</v>
       </c>
       <c r="O33" s="19">
         <v>44744401.881163746</v>
@@ -25114,13 +25114,13 @@
         <v>86070320.273206726</v>
       </c>
       <c r="L34" s="19">
-        <v>55364994.129557326</v>
+        <v>56136772.765589304</v>
       </c>
       <c r="M34" s="19">
-        <v>121748625.07450631</v>
+        <v>123445780.27656218</v>
       </c>
       <c r="N34" s="19">
-        <v>198788359.17682484</v>
+        <v>201559435.21713853</v>
       </c>
       <c r="O34" s="19">
         <v>44926230.686767519</v>
@@ -25294,13 +25294,13 @@
         <v>86220575.189812049</v>
       </c>
       <c r="L35" s="19">
-        <v>55538904.251606762</v>
+        <v>56294682.600095049</v>
       </c>
       <c r="M35" s="19">
-        <v>122375563.20320831</v>
+        <v>124040860.7509245</v>
       </c>
       <c r="N35" s="19">
-        <v>199412784.56239519</v>
+        <v>202126411.4697834</v>
       </c>
       <c r="O35" s="19">
         <v>45108798.394069776</v>
@@ -25474,13 +25474,13 @@
         <v>86371092.409844294</v>
       </c>
       <c r="L36" s="19">
-        <v>55713360.652600631</v>
+        <v>56453036.626787201</v>
       </c>
       <c r="M36" s="19">
-        <v>123005729.71676461</v>
+        <v>124638809.8593557</v>
       </c>
       <c r="N36" s="19">
-        <v>200039171.36594674</v>
+        <v>202694982.59726357</v>
       </c>
       <c r="O36" s="19">
         <v>45292108.005761519</v>
@@ -25654,13 +25654,13 @@
         <v>86521872.391212523</v>
       </c>
       <c r="L37" s="19">
-        <v>55888365.048486672</v>
+        <v>56611836.095155388</v>
       </c>
       <c r="M37" s="19">
-        <v>123639141.23957282</v>
+        <v>125239641.43034083</v>
       </c>
       <c r="N37" s="19">
-        <v>200667525.74860069</v>
+        <v>203265153.08587942</v>
       </c>
       <c r="O37" s="19">
         <v>45476162.536735862</v>
@@ -25834,13 +25834,13 @@
         <v>86672915.592625156</v>
       </c>
       <c r="L38" s="19">
-        <v>56063919.160602748</v>
+        <v>56771082.258203983</v>
       </c>
       <c r="M38" s="19">
-        <v>124275814.48163716</v>
+        <v>125843369.35902627</v>
       </c>
       <c r="N38" s="19">
-        <v>201297853.89083144</v>
+        <v>203836927.43455106</v>
       </c>
       <c r="O38" s="19">
         <v>45660965.014137596</v>

</xml_diff>